<commit_message>
Regretion Run SCD0051,SCD0052,SCD0058,SCD0059,SCD0164 dan merapikan code
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_Digisales/SCD0164_Penyesuaian Kriteria Account Plan Asisten Penjualan.xlsx
+++ b/Lib_Repo_Excel/FileExcel_Digisales/SCD0164_Penyesuaian Kriteria Account Plan Asisten Penjualan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\Digisales\Lib_Repo_Excel\FileExcel_Digisales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DigiSales\Lib_Repo_Excel\FileExcel_Digisales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6C35B2-657B-4FA4-A8AB-76F188E9E74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96270427-D31F-4832-9074-44C6B8187E0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
     <t>tappan</t>
   </si>
   <si>
-    <t>2022-Jul-09</t>
+    <t>2022-Aug-04</t>
   </si>
 </sst>
 </file>
@@ -516,7 +516,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>